<commit_message>
tarea hecha y unas dudas
</commit_message>
<xml_diff>
--- a/Pruebas de Escritorio/Prueba de numero binario.xlsx
+++ b/Pruebas de Escritorio/Prueba de numero binario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Luis\Documents\GitProjects\Clases-de-c\Pruebas de Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uliul\Documents\GITproyect\Clases-de-c\Pruebas de Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3DDF15C9-BE40-447C-B34B-5E9236F203F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6DC54F-C5C4-461B-B9CC-8CE6FFC97E2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FFF4B908-6E81-4526-9188-1DE7FCDF3D61}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FFF4B908-6E81-4526-9188-1DE7FCDF3D61}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -391,16 +391,16 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="3.5703125" customWidth="1"/>
+    <col min="2" max="2" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="3.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>0</v>
       </c>
@@ -426,7 +426,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>59</v>
       </c>
@@ -447,11 +447,11 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:G2" si="1">ROUNDDOWN(E2/2,0)</f>
+        <f t="shared" ref="F2" si="1">ROUNDDOWN(E2/2,0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3">
         <f>MOD(A2,2)</f>
         <v>1</v>
@@ -473,7 +473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -481,7 +481,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>59</v>
       </c>
@@ -510,7 +510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6">
         <f>A5-B5*POWER(2,5-B1)</f>
         <v>27</v>

</xml_diff>